<commit_message>
Exportación de documentación a PDF
</commit_message>
<xml_diff>
--- a/public/assets/docs/trim2/mr/Normalización/PruebaNormalización_v3.xlsx
+++ b/public/assets/docs/trim2/mr/Normalización/PruebaNormalización_v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\TPS_FDS-2671339-AutOsiris-SIW7\public\assets\docs\trim2\mr\Normalización\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMBIENTE 314\Desktop\TPS_FDS-2671339-AutOsiris-SIW7\public\assets\docs\trim2\mr\Normalización\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD52D1A-6F4C-45DD-874B-F8299408B541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF01F72-2697-42BD-88E2-DE8B079CD498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{8720A487-6CAC-4BBD-AAF9-6C89C5E616EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8720A487-6CAC-4BBD-AAF9-6C89C5E616EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Prueba Normalización" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>descripcion</t>
   </si>
@@ -178,6 +169,15 @@
   </si>
   <si>
     <t>….</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -567,44 +567,14 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -642,24 +612,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -702,6 +654,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1019,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A143B86-9A8D-4169-9A83-28C309989942}">
-  <dimension ref="B2:M33"/>
+  <dimension ref="B2:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,355 +1034,355 @@
   <sheetData>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
-        <v>1</v>
-      </c>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="9">
         <v>12345</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20">
-        <v>2</v>
-      </c>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="10">
+        <v>2</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="13">
         <v>12345</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="J11" s="10" t="s">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="J11" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="33"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="26" t="s">
+      <c r="K12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="M12" s="27"/>
+      <c r="M12" s="35"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
-        <v>1</v>
-      </c>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="17">
-        <v>2</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="14">
         <v>5000</v>
       </c>
-      <c r="J13" s="16">
-        <v>1</v>
-      </c>
-      <c r="K13" s="17" t="s">
+      <c r="J13" s="6">
+        <v>1</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="M13" s="29"/>
+      <c r="M13" s="37"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
-        <v>2</v>
-      </c>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="6">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="17">
-        <v>1</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="14">
         <v>3500</v>
       </c>
-      <c r="J14" s="16">
-        <v>2</v>
-      </c>
-      <c r="K14" s="17" t="s">
+      <c r="J14" s="6">
+        <v>2</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="L14" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="M14" s="29"/>
+      <c r="M14" s="37"/>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="20">
+      <c r="B15" s="10">
         <v>3</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="11">
         <v>3</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="15">
         <v>2400</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="10">
         <v>3</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="30" t="s">
+      <c r="L15" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="31"/>
+      <c r="M15" s="39"/>
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="10" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="12"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="13" t="s">
+      <c r="E18" s="1"/>
+      <c r="F18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J18" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="16">
-        <v>1</v>
-      </c>
-      <c r="C19" s="34">
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="18">
         <v>44958</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="14">
         <v>5600</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="16">
-        <v>1</v>
-      </c>
-      <c r="G19" s="17">
-        <v>1</v>
-      </c>
-      <c r="H19" s="17">
-        <v>1</v>
-      </c>
-      <c r="I19" s="17">
+      <c r="E19" s="1"/>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7">
+        <v>1</v>
+      </c>
+      <c r="I19" s="7">
         <v>4</v>
       </c>
-      <c r="J19" s="32">
+      <c r="J19" s="16">
         <v>5000</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="16">
-        <v>2</v>
-      </c>
-      <c r="C20" s="34">
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="18">
         <v>44958</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="14">
         <v>14000</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="16">
-        <v>2</v>
-      </c>
-      <c r="G20" s="17">
-        <v>1</v>
-      </c>
-      <c r="H20" s="17">
-        <v>2</v>
-      </c>
-      <c r="I20" s="17">
-        <v>1</v>
-      </c>
-      <c r="J20" s="32">
+      <c r="E20" s="1"/>
+      <c r="F20" s="6">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7">
+        <v>2</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1</v>
+      </c>
+      <c r="J20" s="16">
         <v>3500</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="20">
+      <c r="B21" s="10">
         <v>3</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="19">
         <v>44958</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="15">
         <v>2000</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="20">
+      <c r="E21" s="1"/>
+      <c r="F21" s="10">
         <v>3</v>
       </c>
-      <c r="G21" s="21">
-        <v>1</v>
-      </c>
-      <c r="H21" s="21">
+      <c r="G21" s="11">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11">
         <v>3</v>
       </c>
-      <c r="I21" s="21">
-        <v>2</v>
-      </c>
-      <c r="J21" s="33">
+      <c r="I21" s="11">
+        <v>2</v>
+      </c>
+      <c r="J21" s="17">
         <v>2400</v>
       </c>
     </row>
@@ -1398,171 +1395,176 @@
     </row>
     <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="G24" s="10" t="s">
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="G24" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="12"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="13" t="s">
+      <c r="E25" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="39">
-        <v>1</v>
-      </c>
-      <c r="C26" s="40">
+      <c r="B26" s="23">
+        <v>1</v>
+      </c>
+      <c r="C26" s="24">
         <v>44958</v>
       </c>
-      <c r="D26" s="41">
-        <v>1</v>
-      </c>
-      <c r="E26" s="42">
-        <v>1</v>
-      </c>
-      <c r="G26" s="16">
-        <v>1</v>
-      </c>
-      <c r="H26" s="17">
-        <v>1</v>
-      </c>
-      <c r="I26" s="17">
-        <v>1</v>
-      </c>
-      <c r="J26" s="19">
+      <c r="D26" s="25">
+        <v>1</v>
+      </c>
+      <c r="E26" s="26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I26" s="7">
+        <v>1</v>
+      </c>
+      <c r="J26" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="39">
-        <v>2</v>
-      </c>
-      <c r="C27" s="40">
+      <c r="B27" s="23">
+        <v>2</v>
+      </c>
+      <c r="C27" s="24">
         <v>44958</v>
       </c>
-      <c r="D27" s="41">
-        <v>1</v>
-      </c>
-      <c r="E27" s="42">
-        <v>1</v>
-      </c>
-      <c r="G27" s="16">
-        <v>2</v>
-      </c>
-      <c r="H27" s="17">
-        <v>1</v>
-      </c>
-      <c r="I27" s="17">
+      <c r="D27" s="25">
+        <v>1</v>
+      </c>
+      <c r="E27" s="26">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>2</v>
+      </c>
+      <c r="H27" s="7">
+        <v>1</v>
+      </c>
+      <c r="I27" s="7">
         <v>3</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="43">
+      <c r="B28" s="27">
         <v>3</v>
       </c>
-      <c r="C28" s="44">
+      <c r="C28" s="28">
         <v>44958</v>
       </c>
-      <c r="D28" s="45">
-        <v>2</v>
-      </c>
-      <c r="E28" s="46">
-        <v>1</v>
-      </c>
-      <c r="G28" s="20">
+      <c r="D28" s="29">
+        <v>2</v>
+      </c>
+      <c r="E28" s="30">
+        <v>1</v>
+      </c>
+      <c r="G28" s="10">
         <v>3</v>
       </c>
-      <c r="H28" s="21">
-        <v>2</v>
-      </c>
-      <c r="I28" s="21">
-        <v>2</v>
-      </c>
-      <c r="J28" s="23">
+      <c r="H28" s="11">
+        <v>2</v>
+      </c>
+      <c r="I28" s="11">
+        <v>2</v>
+      </c>
+      <c r="J28" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="33"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="38" t="s">
+      <c r="B31" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="22" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="39">
-        <v>1</v>
-      </c>
-      <c r="C32" s="41" t="s">
+      <c r="B32" s="23">
+        <v>1</v>
+      </c>
+      <c r="C32" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="26" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="43">
-        <v>2</v>
-      </c>
-      <c r="C33" s="45" t="s">
+      <c r="B33" s="27">
+        <v>2</v>
+      </c>
+      <c r="C33" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="30" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
     <mergeCell ref="F17:J17"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="B3:L4"/>
@@ -1571,12 +1573,17 @@
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="G24:J24"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" xr:uid="{04DBFA0D-0369-422E-9EEA-38458E5E39D9}"/>
     <hyperlink ref="D9" r:id="rId2" xr:uid="{9CC47E0F-073B-4BE1-ABD4-2792CC853DF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>